<commit_message>
Added Evaluation Of Branches
</commit_message>
<xml_diff>
--- a/THUMB_Instructions.xlsx
+++ b/THUMB_Instructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\GBA_Assembler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E0FE9E-927F-4475-B526-C0407C56205F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006A38EC-5570-4184-ABD2-FD8A1C87E05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5DD5E055-AF94-4219-9427-6255363B1F37}"/>
   </bookViews>
@@ -1119,8 +1119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEF809C1-94BC-4152-9D78-FAC92B52A825}">
   <dimension ref="A2:U82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4587,6 +4587,122 @@
     </row>
   </sheetData>
   <mergeCells count="138">
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="P5:R5"/>
+    <mergeCell ref="C2:R2"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="K9:R9"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K10:R10"/>
+    <mergeCell ref="L11:R11"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="P12:R12"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="P7:R7"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="P8:R8"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:R18"/>
+    <mergeCell ref="M19:O19"/>
+    <mergeCell ref="H13:L13"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="P13:R13"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="P14:R14"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="K15:R15"/>
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="P20:R20"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="K21:R21"/>
+    <mergeCell ref="P22:R22"/>
+    <mergeCell ref="M22:O22"/>
+    <mergeCell ref="H16:R16"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="H26:L26"/>
+    <mergeCell ref="M26:O26"/>
+    <mergeCell ref="P26:R26"/>
+    <mergeCell ref="J27:L27"/>
+    <mergeCell ref="M27:O27"/>
+    <mergeCell ref="P27:R27"/>
+    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="P23:R23"/>
+    <mergeCell ref="P24:R24"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="H25:J25"/>
+    <mergeCell ref="K25:R25"/>
+    <mergeCell ref="J31:L31"/>
+    <mergeCell ref="M31:O31"/>
+    <mergeCell ref="P31:R31"/>
+    <mergeCell ref="H32:L32"/>
+    <mergeCell ref="M32:O32"/>
+    <mergeCell ref="P32:R32"/>
+    <mergeCell ref="H28:J28"/>
+    <mergeCell ref="K28:R28"/>
+    <mergeCell ref="H29:J29"/>
+    <mergeCell ref="K29:R29"/>
+    <mergeCell ref="H30:L30"/>
+    <mergeCell ref="M30:O30"/>
+    <mergeCell ref="P30:R30"/>
+    <mergeCell ref="J35:L35"/>
+    <mergeCell ref="M35:O35"/>
+    <mergeCell ref="P35:R35"/>
+    <mergeCell ref="H36:L36"/>
+    <mergeCell ref="M36:O36"/>
+    <mergeCell ref="P36:R36"/>
+    <mergeCell ref="J33:L33"/>
+    <mergeCell ref="M33:O33"/>
+    <mergeCell ref="P33:R33"/>
+    <mergeCell ref="J34:L34"/>
+    <mergeCell ref="M34:O34"/>
+    <mergeCell ref="P34:R34"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="K40:R40"/>
+    <mergeCell ref="M41:O41"/>
+    <mergeCell ref="P41:R41"/>
+    <mergeCell ref="M42:O42"/>
+    <mergeCell ref="P42:R42"/>
+    <mergeCell ref="M37:O37"/>
+    <mergeCell ref="P37:R37"/>
+    <mergeCell ref="H38:L38"/>
+    <mergeCell ref="M38:O38"/>
+    <mergeCell ref="P38:R38"/>
+    <mergeCell ref="M39:O39"/>
+    <mergeCell ref="P39:R39"/>
+    <mergeCell ref="M46:O46"/>
+    <mergeCell ref="P46:R46"/>
+    <mergeCell ref="K47:R47"/>
+    <mergeCell ref="K48:R48"/>
+    <mergeCell ref="M49:O49"/>
+    <mergeCell ref="P49:R49"/>
+    <mergeCell ref="M43:O43"/>
+    <mergeCell ref="P43:R43"/>
+    <mergeCell ref="M44:O44"/>
+    <mergeCell ref="P44:R44"/>
+    <mergeCell ref="M45:O45"/>
+    <mergeCell ref="P45:R45"/>
+    <mergeCell ref="J53:L53"/>
+    <mergeCell ref="M53:O53"/>
+    <mergeCell ref="P53:R53"/>
+    <mergeCell ref="H54:J54"/>
+    <mergeCell ref="K54:R54"/>
+    <mergeCell ref="H55:L55"/>
+    <mergeCell ref="M55:O55"/>
+    <mergeCell ref="P55:R55"/>
+    <mergeCell ref="M50:O50"/>
+    <mergeCell ref="P50:R50"/>
+    <mergeCell ref="H51:J51"/>
+    <mergeCell ref="K51:R51"/>
+    <mergeCell ref="H52:L52"/>
+    <mergeCell ref="M52:O52"/>
+    <mergeCell ref="P52:R52"/>
     <mergeCell ref="C66:F66"/>
     <mergeCell ref="M64:O64"/>
     <mergeCell ref="P64:R64"/>
@@ -4609,122 +4725,6 @@
     <mergeCell ref="M58:O58"/>
     <mergeCell ref="P58:R58"/>
     <mergeCell ref="K63:R63"/>
-    <mergeCell ref="J53:L53"/>
-    <mergeCell ref="M53:O53"/>
-    <mergeCell ref="P53:R53"/>
-    <mergeCell ref="H54:J54"/>
-    <mergeCell ref="K54:R54"/>
-    <mergeCell ref="H55:L55"/>
-    <mergeCell ref="M55:O55"/>
-    <mergeCell ref="P55:R55"/>
-    <mergeCell ref="M50:O50"/>
-    <mergeCell ref="P50:R50"/>
-    <mergeCell ref="H51:J51"/>
-    <mergeCell ref="K51:R51"/>
-    <mergeCell ref="H52:L52"/>
-    <mergeCell ref="M52:O52"/>
-    <mergeCell ref="P52:R52"/>
-    <mergeCell ref="M46:O46"/>
-    <mergeCell ref="P46:R46"/>
-    <mergeCell ref="K47:R47"/>
-    <mergeCell ref="K48:R48"/>
-    <mergeCell ref="M49:O49"/>
-    <mergeCell ref="P49:R49"/>
-    <mergeCell ref="M43:O43"/>
-    <mergeCell ref="P43:R43"/>
-    <mergeCell ref="M44:O44"/>
-    <mergeCell ref="P44:R44"/>
-    <mergeCell ref="M45:O45"/>
-    <mergeCell ref="P45:R45"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="K40:R40"/>
-    <mergeCell ref="M41:O41"/>
-    <mergeCell ref="P41:R41"/>
-    <mergeCell ref="M42:O42"/>
-    <mergeCell ref="P42:R42"/>
-    <mergeCell ref="M37:O37"/>
-    <mergeCell ref="P37:R37"/>
-    <mergeCell ref="H38:L38"/>
-    <mergeCell ref="M38:O38"/>
-    <mergeCell ref="P38:R38"/>
-    <mergeCell ref="M39:O39"/>
-    <mergeCell ref="P39:R39"/>
-    <mergeCell ref="J35:L35"/>
-    <mergeCell ref="M35:O35"/>
-    <mergeCell ref="P35:R35"/>
-    <mergeCell ref="H36:L36"/>
-    <mergeCell ref="M36:O36"/>
-    <mergeCell ref="P36:R36"/>
-    <mergeCell ref="J33:L33"/>
-    <mergeCell ref="M33:O33"/>
-    <mergeCell ref="P33:R33"/>
-    <mergeCell ref="J34:L34"/>
-    <mergeCell ref="M34:O34"/>
-    <mergeCell ref="P34:R34"/>
-    <mergeCell ref="J31:L31"/>
-    <mergeCell ref="M31:O31"/>
-    <mergeCell ref="P31:R31"/>
-    <mergeCell ref="H32:L32"/>
-    <mergeCell ref="M32:O32"/>
-    <mergeCell ref="P32:R32"/>
-    <mergeCell ref="H28:J28"/>
-    <mergeCell ref="K28:R28"/>
-    <mergeCell ref="H29:J29"/>
-    <mergeCell ref="K29:R29"/>
-    <mergeCell ref="H30:L30"/>
-    <mergeCell ref="M30:O30"/>
-    <mergeCell ref="P30:R30"/>
-    <mergeCell ref="H26:L26"/>
-    <mergeCell ref="M26:O26"/>
-    <mergeCell ref="P26:R26"/>
-    <mergeCell ref="J27:L27"/>
-    <mergeCell ref="M27:O27"/>
-    <mergeCell ref="P27:R27"/>
-    <mergeCell ref="M23:O23"/>
-    <mergeCell ref="P23:R23"/>
-    <mergeCell ref="P24:R24"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="H25:J25"/>
-    <mergeCell ref="K25:R25"/>
-    <mergeCell ref="M20:O20"/>
-    <mergeCell ref="P20:R20"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="K21:R21"/>
-    <mergeCell ref="P22:R22"/>
-    <mergeCell ref="M22:O22"/>
-    <mergeCell ref="H16:R16"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H18:R18"/>
-    <mergeCell ref="M19:O19"/>
-    <mergeCell ref="H13:L13"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="P13:R13"/>
-    <mergeCell ref="M14:O14"/>
-    <mergeCell ref="P14:R14"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="K15:R15"/>
-    <mergeCell ref="L11:R11"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="P12:R12"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="K6:R6"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="P7:R7"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="P8:R8"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="P4:R4"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="P5:R5"/>
-    <mergeCell ref="C2:R2"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="K9:R9"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:R10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>